<commit_message>
calculates number of months per harvest and average number of harvest cycles
</commit_message>
<xml_diff>
--- a/economic/economic_parameters_full.xlsx
+++ b/economic/economic_parameters_full.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1240" windowWidth="43840" windowHeight="18620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="18060" yWindow="2360" windowWidth="43840" windowHeight="18620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1114,6 +1114,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1338,94 +1341,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>2.26226879442062</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1830073641479</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.43024777734444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.45680991885675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.57942076407755</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.07264166616427</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.63501532626281</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.61960928418567</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.43024777734444</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.75305748314349</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.63501532626281</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.45680991885675</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.60946254612797</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.87189650426955</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.57786510138361</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.26226879442062</c:v>
+                  <c:v>2.78742889426042</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.57942076407755</c:v>
+                  <c:v>2.69228330336334</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.23995659555028</c:v>
+                  <c:v>2.25780635464655</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.22133653435016</c:v>
+                  <c:v>2.67831161692787</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2803576127905</c:v>
+                  <c:v>2.62800292090356</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2.63018101650757</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.07264166616427</c:v>
+                  <c:v>3.01055088296379</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1830073641479</c:v>
+                  <c:v>2.78979292485501</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.69228330336334</c:v>
+                  <c:v>2.23995659555028</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>2.46722227832957</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.67852411405996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.22133653435016</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.75289811029442</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.22834893970941</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.56430690555705</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.87189650426955</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>2.38121406411273</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="25">
+                  <c:v>3.57786510138361</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.60946254612797</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>2.47399562441521</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.67852411405996</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.46722227832957</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.25780635464655</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.22834893970941</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.78742889426042</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.56430690555705</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.75289811029442</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.78979292485501</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.62800292090356</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.67831161692787</c:v>
+                  <c:v>2.2803576127905</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.01055088296379</c:v>
+                  <c:v>2.75305748314349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,11 +1443,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1086606064"/>
-        <c:axId val="1086207616"/>
+        <c:axId val="634256272"/>
+        <c:axId val="640986784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1086606064"/>
+        <c:axId val="634256272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1500,12 +1503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1086207616"/>
+        <c:crossAx val="640986784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1086207616"/>
+        <c:axId val="640986784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1564,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1086606064"/>
+        <c:crossAx val="634256272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3955,8 +3958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:G61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3993,7 +3996,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="61" t="s">
         <v>95</v>
       </c>
@@ -4014,7 +4017,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
@@ -4090,7 +4093,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="160" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -4266,7 +4269,7 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C26" s="22"/>
     </row>
-    <row r="31" spans="1:7" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="61" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="82" t="s">
         <v>0</v>
       </c>
@@ -4885,92 +4888,92 @@
     </row>
     <row r="65" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="81" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B65" s="85">
-        <v>4.3141042594369097</v>
+        <v>4.5267044817054201</v>
       </c>
       <c r="C65" s="85">
-        <v>2.7154984052125601</v>
+        <v>1.56434048086624</v>
       </c>
       <c r="D65" s="85">
-        <v>3.3549407469023</v>
+        <v>2.7492860812019102</v>
       </c>
       <c r="E65">
-        <v>2.6196092841856702</v>
+        <v>2.2622687944206201</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" s="84">
-        <v>4.7701719312275097</v>
+        <v>3.9361410720882799</v>
       </c>
       <c r="C66" s="84">
-        <v>1.94194161515668</v>
+        <v>1.7174969059002201</v>
       </c>
       <c r="D66" s="84">
-        <v>3.0732337415850099</v>
+        <v>2.6049545723754401</v>
       </c>
       <c r="E66">
-        <v>2.43024777734444</v>
+        <v>2.1830073641479002</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B67" s="84">
-        <v>4.1068727794053501</v>
-      </c>
-      <c r="C67" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="D67" s="90">
-        <v>3.0105508829637899</v>
+        <v>4.7701719312275097</v>
+      </c>
+      <c r="C67" s="84">
+        <v>1.94194161515668</v>
+      </c>
+      <c r="D67" s="84">
+        <v>3.0732337415850099</v>
       </c>
       <c r="E67">
-        <v>2.7530574831434902</v>
+        <v>2.43024777734444</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B68" s="85" t="s">
-        <v>110</v>
+        <v>17</v>
+      </c>
+      <c r="B68" s="85">
+        <v>3.9559041174404799</v>
       </c>
       <c r="C68" s="85">
-        <v>3.4788586475789498</v>
-      </c>
-      <c r="D68" s="91">
-        <v>2.8718965042695501</v>
+        <v>2.0205589892941802</v>
+      </c>
+      <c r="D68" s="85">
+        <v>2.7946970405527001</v>
       </c>
       <c r="E68">
-        <v>2.6350153262628102</v>
+        <v>2.45680991885675</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B69" s="84">
-        <v>3.9559041174404799</v>
+        <v>4.5368821292775703</v>
       </c>
       <c r="C69" s="84">
-        <v>2.0205589892941802</v>
+        <v>1.51645984310309</v>
       </c>
       <c r="D69" s="84">
-        <v>2.7946970405527001</v>
+        <v>2.72462875757288</v>
       </c>
       <c r="E69">
-        <v>2.45680991885675</v>
+        <v>2.5794207640775499</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="B70" s="84" t="s">
         <v>110</v>
@@ -4979,129 +4982,129 @@
         <v>110</v>
       </c>
       <c r="D70" s="90">
-        <v>2.7897929248550102</v>
+        <v>2.6094625461279701</v>
       </c>
       <c r="E70">
-        <v>2.6094625461279701</v>
+        <v>2.0726416661642699</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B71" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="84" t="s">
-        <v>110</v>
+      <c r="C71" s="84">
+        <v>3.4788586475789498</v>
       </c>
       <c r="D71" s="90">
-        <v>2.7874288942604202</v>
+        <v>2.8718965042695501</v>
       </c>
       <c r="E71">
-        <v>2.8718965042695501</v>
+        <v>2.6350153262628102</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="D72" s="91">
-        <v>2.7528981102944199</v>
+        <v>21</v>
+      </c>
+      <c r="B72" s="85">
+        <v>4.3141042594369097</v>
+      </c>
+      <c r="C72" s="85">
+        <v>2.7154984052125601</v>
+      </c>
+      <c r="D72" s="85">
+        <v>3.3549407469023</v>
       </c>
       <c r="E72">
-        <v>3.57786510138361</v>
+        <v>2.6196092841856702</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B73" s="84">
-        <v>4.5267044817054201</v>
-      </c>
-      <c r="C73" s="84">
-        <v>1.56434048086624</v>
-      </c>
-      <c r="D73" s="85">
-        <v>2.7492860812019102</v>
+        <v>2.4179128348660499</v>
+      </c>
+      <c r="C73" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="91">
+        <v>2.2622687944206201</v>
       </c>
       <c r="E73">
-        <v>2.2622687944206201</v>
+        <v>2.7874288942604202</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B74" s="84">
-        <v>4.5368821292775703</v>
+        <v>117</v>
+      </c>
+      <c r="B74" s="84" t="s">
+        <v>110</v>
       </c>
       <c r="C74" s="84">
-        <v>1.51645984310309</v>
-      </c>
-      <c r="D74" s="92">
-        <v>2.72462875757288</v>
+        <v>1.7526413346306</v>
+      </c>
+      <c r="D74" s="101">
+        <v>2.5794207640775499</v>
       </c>
       <c r="E74">
-        <v>2.5794207640775499</v>
+        <v>2.69228330336334</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B75" s="84">
-        <v>4.5066321456208396</v>
-      </c>
-      <c r="C75" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" s="90">
-        <v>2.69228330336334</v>
+        <v>3.85469392471148</v>
+      </c>
+      <c r="C75" s="84">
+        <v>1.3048491019189099</v>
+      </c>
+      <c r="D75" s="84">
+        <v>2.3247870310359402</v>
       </c>
       <c r="E75">
-        <v>2.23995659555028</v>
+        <v>2.2578063546465499</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B76" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="85" t="s">
-        <v>110</v>
-      </c>
-      <c r="D76" s="91">
-        <v>2.67852411405996</v>
+        <v>25</v>
+      </c>
+      <c r="B76" s="85">
+        <v>2.4515274954656898</v>
+      </c>
+      <c r="C76" s="85">
+        <v>1.6210698394699301</v>
+      </c>
+      <c r="D76" s="85">
+        <v>1.9532529018682401</v>
       </c>
       <c r="E76">
-        <v>2.2213365343501601</v>
+        <v>2.67831161692787</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="C77" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="D77" s="90">
-        <v>2.67831161692787</v>
+        <v>26</v>
+      </c>
+      <c r="B77" s="84">
+        <v>3.34013466856603</v>
+      </c>
+      <c r="C77" s="84">
+        <v>1.3939621337938899</v>
+      </c>
+      <c r="D77" s="84">
+        <v>2.17243114770275</v>
       </c>
       <c r="E77">
-        <v>2.2803576127905001</v>
+        <v>2.62800292090356</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -5123,279 +5126,283 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B79" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="C79" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="D79" s="90">
-        <v>2.6094625461279701</v>
+        <v>28</v>
+      </c>
+      <c r="B79" s="84">
+        <v>1.0479087452471501</v>
+      </c>
+      <c r="C79" s="84">
+        <v>2.4034376593746298</v>
+      </c>
+      <c r="D79" s="84">
+        <v>1.86122609372364</v>
       </c>
       <c r="E79">
-        <v>2.0726416661642699</v>
+        <v>3.0105508829637899</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B80" s="85">
-        <v>3.9361410720882799</v>
+        <v>2.6498560119678398</v>
       </c>
       <c r="C80" s="85">
-        <v>1.7174969059002201</v>
+        <v>1.8845356556252999</v>
       </c>
       <c r="D80" s="85">
-        <v>2.6049545723754401</v>
+        <v>2.19066379816232</v>
       </c>
       <c r="E80">
-        <v>2.1830073641479002</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.7897929248550102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B81" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="84">
+        <v>4.5066321456208396</v>
+      </c>
+      <c r="C81" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C81" s="84">
-        <v>1.7526413346306</v>
-      </c>
-      <c r="D81" s="80">
-        <v>2.5794207640775499</v>
+      <c r="D81" s="90">
+        <v>2.69228330336334</v>
       </c>
       <c r="E81">
-        <v>2.69228330336334</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.23995659555028</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B82" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C82" s="84" t="s">
+      <c r="C82" s="84">
+        <v>1.45174676515912</v>
+      </c>
+      <c r="D82" s="90">
+        <v>2.3812140641127302</v>
+      </c>
+      <c r="E82">
+        <v>2.4672222783295701</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83" s="84">
+        <v>3.8061526111988702</v>
+      </c>
+      <c r="C83" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="D82" s="90">
-        <v>2.56430690555705</v>
-      </c>
-      <c r="E82">
-        <v>2.3812140641127302</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B83" s="84">
-        <v>2.7114526660818599</v>
-      </c>
-      <c r="C83" s="84">
-        <v>2.3764566111488898</v>
-      </c>
-      <c r="D83" s="84">
-        <v>2.5104550331220801</v>
+      <c r="D83" s="90">
+        <v>2.4739956244152101</v>
       </c>
       <c r="E83">
-        <v>2.4739956244152101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.67852411405996</v>
+      </c>
+      <c r="H83">
+        <f>190/2</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B84" s="85">
-        <v>3.8061526111988702</v>
+        <v>33</v>
+      </c>
+      <c r="B84" s="85" t="s">
+        <v>110</v>
       </c>
       <c r="C84" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D84" s="90">
-        <v>2.4739956244152101</v>
+        <v>2.67852411405996</v>
       </c>
       <c r="E84">
-        <v>2.67852411405996</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.2213365343501601</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B85" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" s="84">
+        <v>3.31395831021204</v>
+      </c>
+      <c r="C85" s="84">
+        <v>1.45899039411242</v>
+      </c>
+      <c r="D85" s="84">
+        <v>2.2009775605522699</v>
+      </c>
+      <c r="E85">
+        <v>2.7528981102944199</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="84">
+        <v>3.5730892129840099</v>
+      </c>
+      <c r="C86" s="84">
+        <v>1.46361004418082</v>
+      </c>
+      <c r="D86" s="84">
+        <v>2.3074017117021</v>
+      </c>
+      <c r="E86">
+        <v>2.2283489397094098</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C85" s="84">
-        <v>1.45174676515912</v>
-      </c>
-      <c r="D85" s="90">
-        <v>2.3812140641127302</v>
-      </c>
-      <c r="E85">
-        <v>2.4672222783295701</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B86" s="84">
-        <v>3.85469392471148</v>
-      </c>
-      <c r="C86" s="84">
-        <v>1.3048491019189099</v>
-      </c>
-      <c r="D86" s="84">
-        <v>2.3247870310359402</v>
-      </c>
-      <c r="E86">
-        <v>2.2578063546465499</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A87" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B87" s="84">
-        <v>3.5730892129840099</v>
-      </c>
       <c r="C87" s="84">
-        <v>1.46361004418082</v>
-      </c>
-      <c r="D87" s="84">
-        <v>2.3074017117021</v>
+        <v>1.2686055032766601</v>
+      </c>
+      <c r="D87" s="90">
+        <v>2.2283489397094098</v>
       </c>
       <c r="E87">
-        <v>2.2283489397094098</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.56430690555705</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B88" s="85">
-        <v>2.4179128348660499</v>
+        <v>37</v>
+      </c>
+      <c r="B88" s="85" t="s">
+        <v>110</v>
       </c>
       <c r="C88" s="85" t="s">
         <v>110</v>
       </c>
       <c r="D88" s="90">
-        <v>2.2622687944206201</v>
+        <v>2.7874288942604202</v>
       </c>
       <c r="E88">
-        <v>2.7874288942604202</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.8718965042695501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B89" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="84">
-        <v>1.2686055032766601</v>
+      <c r="C89" s="84" t="s">
+        <v>110</v>
       </c>
       <c r="D89" s="90">
-        <v>2.2283489397094098</v>
+        <v>2.56430690555705</v>
       </c>
       <c r="E89">
-        <v>2.56430690555705</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.3812140641127302</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B90" s="84">
-        <v>3.31395831021204</v>
-      </c>
-      <c r="C90" s="84">
-        <v>1.45899039411242</v>
-      </c>
-      <c r="D90" s="84">
-        <v>2.2009775605522699</v>
+        <v>39</v>
+      </c>
+      <c r="B90" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D90" s="90">
+        <v>2.7528981102944199</v>
       </c>
       <c r="E90">
-        <v>2.7528981102944199</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3.57786510138361</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B91" s="84">
-        <v>2.6498560119678398</v>
-      </c>
-      <c r="C91" s="84">
-        <v>1.8845356556252999</v>
-      </c>
-      <c r="D91" s="84">
-        <v>2.19066379816232</v>
+        <v>40</v>
+      </c>
+      <c r="B91" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D91" s="90">
+        <v>2.7897929248550102</v>
       </c>
       <c r="E91">
-        <v>2.7897929248550102</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.6094625461279701</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B92" s="85">
-        <v>3.34013466856603</v>
+        <v>2.7114526660818599</v>
       </c>
       <c r="C92" s="85">
-        <v>1.3939621337938899</v>
+        <v>2.3764566111488898</v>
       </c>
       <c r="D92" s="85">
-        <v>2.17243114770275</v>
+        <v>2.5104550331220801</v>
       </c>
       <c r="E92">
-        <v>2.62800292090356</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.4739956244152101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B93" s="84">
-        <v>2.4515274954656898</v>
-      </c>
-      <c r="C93" s="84">
-        <v>1.6210698394699301</v>
-      </c>
-      <c r="D93" s="84">
-        <v>1.9532529018682401</v>
+        <v>42</v>
+      </c>
+      <c r="B93" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="D93" s="90">
+        <v>2.67831161692787</v>
       </c>
       <c r="E93">
-        <v>2.67831161692787</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.2803576127905001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="34" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B94" s="92">
-        <v>1.0479087452471501</v>
-      </c>
-      <c r="C94" s="92">
-        <v>2.4034376593746298</v>
-      </c>
-      <c r="D94" s="84">
-        <v>1.86122609372364</v>
+        <v>4.1068727794053501</v>
+      </c>
+      <c r="C94" s="92" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" s="90">
+        <v>3.0105508829637899</v>
       </c>
       <c r="E94">
-        <v>3.0105508829637899</v>
+        <v>2.7530574831434902</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A65:D94">
-    <sortCondition descending="1" ref="D65:D94"/>
+  <sortState ref="A65:E94">
+    <sortCondition ref="A65:A94"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>